<commit_message>
:hammer: Push Lolos UAT
</commit_message>
<xml_diff>
--- a/Prototype/ad.xlsx
+++ b/Prototype/ad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marissanuramalia/Desktop/Coolyeah/Repositories/GitHub/sparx-ea-diagram-generator/Prototype/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82D5D2CE-294A-3C46-A931-7AA64BEAA504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E971E41C-CCDA-EB4E-9809-72754EC97343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{E8BE6E05-19F7-B340-BD02-A47EA5B276F1}"/>
+    <workbookView xWindow="10280" yWindow="500" windowWidth="18520" windowHeight="15940" xr2:uid="{E8BE6E05-19F7-B340-BD02-A47EA5B276F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>UC ID</t>
-  </si>
-  <si>
-    <t>UC-01-01</t>
-  </si>
-  <si>
-    <t>SS-01</t>
-  </si>
-  <si>
-    <t>UC-01</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Proses 1</t>
   </si>
@@ -59,15 +44,6 @@
     <t>HCMS</t>
   </si>
   <si>
-    <t>Subsistem 1</t>
-  </si>
-  <si>
-    <t>Modul 1</t>
-  </si>
-  <si>
-    <t>Lane</t>
-  </si>
-  <si>
     <t>Approver</t>
   </si>
   <si>
@@ -80,29 +56,26 @@
     <t>3: Menekan tombol B</t>
   </si>
   <si>
-    <t>4: Gateway, Apakah ABC?</t>
-  </si>
-  <si>
-    <t>4.1.1: Ya, Menampilkan AB</t>
-  </si>
-  <si>
-    <t>4.2.1: Tidak, Menampilkan Warning</t>
-  </si>
-  <si>
-    <t>4.1.2: Menekan tombol</t>
-  </si>
-  <si>
-    <t>4.1.2: Menampilkan Sukses</t>
-  </si>
-  <si>
-    <t>5: End</t>
+    <t>4: Menampilkan C</t>
+  </si>
+  <si>
+    <t>5: Menekan Tombol "Save"</t>
+  </si>
+  <si>
+    <t>6: Menyimpan A</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>start</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,13 +83,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,9 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,103 +448,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF9BAF8-C4E6-D146-90F8-B001EBBDC655}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>